<commit_message>
botões de inserir e remover banco
implementação dos botões de inserir e remover banco
</commit_message>
<xml_diff>
--- a/Organizador de Declaração de Imposto de Renda.xlsx
+++ b/Organizador de Declaração de Imposto de Renda.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikson\Desktop\BootCamp_Santander_Excel_com_IA\Projetos\PJ02 - ORGANIZADOR DE DECLARAÇÃO DE IMPOSTO DE RENDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A9566A1-B3C2-49C8-A2A6-ED129F21FCEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E585B89B-EA40-4334-9728-72289083B0B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="499" activeTab="1" xr2:uid="{8EBFE920-9B91-4499-8E1F-DCFD25697F82}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="391" activeTab="1" xr2:uid="{8EBFE920-9B91-4499-8E1F-DCFD25697F82}"/>
   </bookViews>
   <sheets>
     <sheet name="TÍTULAR" sheetId="1" r:id="rId1"/>
     <sheet name="INFORMES" sheetId="8" r:id="rId2"/>
     <sheet name="NOTAS" sheetId="9" r:id="rId3"/>
-    <sheet name="TABELAS" sheetId="10" state="hidden" r:id="rId4"/>
+    <sheet name="TABELAS" sheetId="10" r:id="rId4"/>
+    <sheet name="_LOG_BANCOS" sheetId="11" state="veryHidden" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="97">
   <si>
     <t>NOME</t>
   </si>
@@ -300,6 +301,36 @@
   </si>
   <si>
     <t>HOLERITE</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>DataHora</t>
+  </si>
+  <si>
+    <t>SheetName</t>
+  </si>
+  <si>
+    <t>DestAddress</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>D3</t>
   </si>
 </sst>
 </file>
@@ -505,7 +536,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -513,30 +544,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="167" fontId="3" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="168" fontId="3" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -569,6 +576,57 @@
     <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="169" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="168" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="168" fontId="3" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hiperlink" xfId="3" builtinId="8"/>
@@ -590,8 +648,25 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
       <numFmt numFmtId="168" formatCode="&quot;R$&quot;\ #,##0.00"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <font>
@@ -607,6 +682,7 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <font>
@@ -622,21 +698,7 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Segoe UI"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <font>
@@ -661,13 +723,13 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFDE1317"/>
       <color rgb="FFB047DF"/>
       <color rgb="FF7516BC"/>
       <color rgb="FF550476"/>
       <color rgb="FFC983E9"/>
       <color rgb="FF212121"/>
       <color rgb="FF3D3D3D"/>
-      <color rgb="FFDE1317"/>
     </mruColors>
   </colors>
   <extLst>
@@ -2236,17 +2298,17 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>390525</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp macro="[0]!INSERIR_NOVO_BANCO" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="2" name="Retângulo 1">
           <a:extLst>
@@ -2259,7 +2321,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10467975" y="1304925"/>
+          <a:off x="10296525" y="1381125"/>
           <a:ext cx="1095375" cy="552450"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2296,6 +2358,83 @@
             </a:rPr>
             <a:t>INSERIR NOVO BANCO</a:t>
           </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="[0]!REMOVER_BANCO" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Retângulo 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3490692-D1FF-F8E4-9478-1F0C2CDA6A59}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10306050" y="2057400"/>
+          <a:ext cx="1095375" cy="552450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="DE1317"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100">
+              <a:latin typeface="SegoeUI"/>
+            </a:rPr>
+            <a:t>REMOVER</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100" baseline="0">
+              <a:latin typeface="SegoeUI"/>
+            </a:rPr>
+            <a:t> BANCO</a:t>
+          </a:r>
+          <a:endParaRPr lang="pt-BR" sz="1100">
+            <a:latin typeface="SegoeUI"/>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -3039,12 +3178,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6D3D7E3C-6E5A-4CE8-9D6C-17A8EBBA39CD}" name="Tabela1" displayName="Tabela1" ref="C8:E19" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6D3D7E3C-6E5A-4CE8-9D6C-17A8EBBA39CD}" name="Tabela1" displayName="Tabela1" ref="C8:E19" totalsRowShown="0" headerRowDxfId="4" dataDxfId="0">
   <autoFilter ref="C8:E19" xr:uid="{6D3D7E3C-6E5A-4CE8-9D6C-17A8EBBA39CD}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{E6E670E1-8698-4872-BCF7-BF2EDAC620E1}" name="DATA" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{A1537E7D-FC27-44BA-A183-6861C3BFD418}" name="CATEGORIA" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{47D71516-2EC3-44CD-B113-80BAFFADEF0E}" name="VALOR" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{E6E670E1-8698-4872-BCF7-BF2EDAC620E1}" name="DATA" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{A1537E7D-FC27-44BA-A183-6861C3BFD418}" name="CATEGORIA" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{47D71516-2EC3-44CD-B113-80BAFFADEF0E}" name="VALOR" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3371,7 +3510,7 @@
   <dimension ref="A3:E19"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="D18" sqref="D18"/>
       <extLst>
         <ext xmlns:xlsdti="http://schemas.microsoft.com/office/spreadsheetml/2023/showDataTypeIcons" uri="{77bfe23e-c014-4d31-8a63-9c772dbf06b6}">
           <xlsdti:showDataTypeIcons visible="0"/>
@@ -3393,18 +3532,18 @@
       <c r="E3" s="4"/>
     </row>
     <row r="4" spans="3:5" ht="22.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
     </row>
     <row r="5" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="3:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C6" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="22" t="s">
         <v>17</v>
       </c>
     </row>
@@ -3412,7 +3551,7 @@
       <c r="C7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="24">
         <v>98765432147</v>
       </c>
     </row>
@@ -3420,7 +3559,7 @@
       <c r="C8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="25">
         <v>34605</v>
       </c>
     </row>
@@ -3428,7 +3567,7 @@
       <c r="C9" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="22">
         <v>87542196</v>
       </c>
     </row>
@@ -3436,7 +3575,7 @@
       <c r="C10" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="22" t="s">
         <v>21</v>
       </c>
     </row>
@@ -3444,7 +3583,7 @@
       <c r="C11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="22" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3452,7 +3591,7 @@
       <c r="C12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="22" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3460,7 +3599,7 @@
       <c r="C13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13" s="26">
         <v>987654321</v>
       </c>
     </row>
@@ -3468,7 +3607,7 @@
       <c r="C14" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="11">
+      <c r="D14" s="27">
         <v>8188923247</v>
       </c>
     </row>
@@ -3476,7 +3615,7 @@
       <c r="C15" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="10">
+      <c r="D15" s="28">
         <v>81988923247</v>
       </c>
     </row>
@@ -3484,7 +3623,7 @@
       <c r="C16" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="29" t="s">
         <v>18</v>
       </c>
     </row>
@@ -3492,7 +3631,7 @@
       <c r="C17" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="22" t="s">
         <v>16</v>
       </c>
     </row>
@@ -3500,7 +3639,7 @@
       <c r="C18" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="22" t="s">
         <v>16</v>
       </c>
     </row>
@@ -3508,11 +3647,12 @@
       <c r="C19" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="22" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="1">
     <mergeCell ref="C4:E4"/>
   </mergeCells>
@@ -3532,10 +3672,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC303DA2-A31C-4F20-9E26-F1BC416EC9D8}">
   <sheetPr codeName="Planilha2"/>
-  <dimension ref="A3:E13"/>
+  <dimension ref="A3:E37"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
       <extLst>
         <ext xmlns:xlsdti="http://schemas.microsoft.com/office/spreadsheetml/2023/showDataTypeIcons" uri="{77bfe23e-c014-4d31-8a63-9c772dbf06b6}">
           <xlsdti:showDataTypeIcons visible="0"/>
@@ -3557,56 +3697,105 @@
       <c r="E3" s="4"/>
     </row>
     <row r="4" spans="2:5" ht="22.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
     </row>
     <row r="5" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="6" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="24" t="e">
-        <f>SUM(D12+#REF!+#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D7" s="25"/>
+      <c r="C7" s="16">
+        <f>SUM(D12,D16,D20,D24,D28)</f>
+        <v>500000</v>
+      </c>
+      <c r="D7" s="17"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="22"/>
+      <c r="B8" s="14"/>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="21"/>
+      <c r="B9" s="13"/>
     </row>
     <row r="11" spans="2:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="22" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="12" spans="2:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="12">
+      <c r="D12" s="23">
         <v>500000</v>
       </c>
     </row>
     <row r="13" spans="2:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="22" t="s">
         <v>78</v>
       </c>
     </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C14" s="31"/>
+      <c r="D14" s="31"/>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C18" s="31"/>
+      <c r="D18" s="31"/>
+    </row>
+    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C22" s="31"/>
+      <c r="D22" s="31"/>
+    </row>
+    <row r="26" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C26" s="31"/>
+      <c r="D26" s="31"/>
+    </row>
+    <row r="30" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
+    </row>
+    <row r="31" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C31" s="31"/>
+      <c r="D31" s="31"/>
+    </row>
+    <row r="32" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C32" s="31"/>
+      <c r="D32" s="31"/>
+    </row>
+    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C33" s="31"/>
+      <c r="D33" s="31"/>
+    </row>
+    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C34" s="31"/>
+      <c r="D34" s="31"/>
+    </row>
+    <row r="35" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C35" s="31"/>
+      <c r="D35" s="31"/>
+    </row>
+    <row r="36" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C36" s="31"/>
+      <c r="D36" s="31"/>
+    </row>
+    <row r="37" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C37" s="31"/>
+      <c r="D37" s="31"/>
+    </row>
   </sheetData>
+  <sheetProtection selectLockedCells="1"/>
   <mergeCells count="2">
     <mergeCell ref="C4:E4"/>
     <mergeCell ref="C7:D7"/>
@@ -3634,7 +3823,7 @@
   <dimension ref="A3:E36"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C10" sqref="C9:C10"/>
       <extLst>
         <ext xmlns:xlsdti="http://schemas.microsoft.com/office/spreadsheetml/2023/showDataTypeIcons" uri="{77bfe23e-c014-4d31-8a63-9c772dbf06b6}">
           <xlsdti:showDataTypeIcons visible="0"/>
@@ -3658,177 +3847,178 @@
       <c r="E3" s="4"/>
     </row>
     <row r="4" spans="3:5" ht="22.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
     </row>
     <row r="7" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
     </row>
     <row r="8" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="E8" s="7" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="9" spans="3:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="C9" s="18">
+      <c r="C9" s="19">
         <v>46061</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="D9" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="E9" s="20">
+      <c r="E9" s="21">
         <v>3000</v>
       </c>
     </row>
     <row r="10" spans="3:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="C10" s="18"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="20"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="21"/>
     </row>
     <row r="11" spans="3:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="C11" s="18"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="20"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="21"/>
     </row>
     <row r="12" spans="3:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="C12" s="18"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="20"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="21"/>
     </row>
     <row r="13" spans="3:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="C13" s="18"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="20"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="21"/>
     </row>
     <row r="14" spans="3:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="C14" s="18"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="20"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="21"/>
     </row>
     <row r="15" spans="3:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="C15" s="18"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="20"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="21"/>
     </row>
     <row r="16" spans="3:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="C16" s="18"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="20"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="21"/>
     </row>
     <row r="17" spans="3:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="C17" s="18"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="20"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="21"/>
     </row>
     <row r="18" spans="3:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="C18" s="18"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="20"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="21"/>
     </row>
     <row r="19" spans="3:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="C19" s="18"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="20"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="21"/>
     </row>
     <row r="20" spans="3:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="C20" s="18"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="20"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="12"/>
     </row>
     <row r="21" spans="3:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="C21" s="18"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="20"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="12"/>
     </row>
     <row r="22" spans="3:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="C22" s="18"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="20"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="12"/>
     </row>
     <row r="23" spans="3:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="C23" s="18"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="20"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="12"/>
     </row>
     <row r="24" spans="3:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="C24" s="18"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="20"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="12"/>
     </row>
     <row r="25" spans="3:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="C25" s="18"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="20"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="12"/>
     </row>
     <row r="26" spans="3:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="C26" s="18"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="20"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="12"/>
     </row>
     <row r="27" spans="3:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="C27" s="18"/>
-      <c r="D27" s="19"/>
-      <c r="E27" s="20"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="12"/>
     </row>
     <row r="28" spans="3:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="C28" s="18"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="20"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="12"/>
     </row>
     <row r="29" spans="3:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="C29" s="18"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="20"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="12"/>
     </row>
     <row r="30" spans="3:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="C30" s="18"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="20"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="12"/>
     </row>
     <row r="31" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C31" s="16"/>
-      <c r="D31" s="16"/>
-      <c r="E31" s="17"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="9"/>
     </row>
     <row r="32" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C32" s="16"/>
-      <c r="D32" s="16"/>
-      <c r="E32" s="17"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="9"/>
     </row>
     <row r="33" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C33" s="16"/>
-      <c r="D33" s="16"/>
-      <c r="E33" s="17"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="9"/>
     </row>
     <row r="34" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C34" s="16"/>
-      <c r="D34" s="16"/>
-      <c r="E34" s="17"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="9"/>
     </row>
     <row r="35" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C35" s="16"/>
-      <c r="D35" s="16"/>
-      <c r="E35" s="17"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="9"/>
     </row>
     <row r="36" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C36" s="16"/>
-      <c r="D36" s="16"/>
-      <c r="E36" s="17"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="9"/>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="2">
     <mergeCell ref="C4:E4"/>
     <mergeCell ref="C7:E7"/>
@@ -3851,7 +4041,7 @@
   <sheetPr codeName="Planilha4"/>
   <dimension ref="A1:A51"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
+    <sheetView topLeftCell="A29" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -3861,7 +4051,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="5" t="s">
         <v>77</v>
       </c>
     </row>
@@ -4113,6 +4303,52 @@
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0B5DCEC-05BD-4F16-B926-58EDC8D07CE9}">
+  <sheetPr codeName="Planilha5"/>
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>